<commit_message>
Current version of analysis files
</commit_message>
<xml_diff>
--- a/FlowRateConversion.xlsx
+++ b/FlowRateConversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sodav\Desktop\BEng\NebuliserAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43616678-8D96-43ED-B19E-DB528A8BFD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B659598-9822-4168-AA73-034C82BA6D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{23D1222D-910B-410A-98F7-A6FBC2477783}"/>
   </bookViews>
@@ -85,6 +85,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF1AC486"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -124,18 +129,22 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Real (Measured)</a:t>
+              <a:t>Measured</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Flow Rate Versus Flow Rate on Pump</a:t>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Flow Rate vs Flow Rate Displayed on Pump</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -143,10 +152,9 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1050" i="1" baseline="0"/>
-              <a:t>Conclusion: Real Flow Rate is 3x Greater Than Indicated by Pump</a:t>
+              <a:rPr lang="en-US" sz="1000" i="1"/>
+              <a:t>Conclusion: Real Flow Rate is 3.2x Greater Than Indicated by Pump</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1050" i="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -170,7 +178,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -211,11 +219,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="1AC486"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="1AC486"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -225,7 +233,7 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="1AC486"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -237,8 +245,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.2472501630937754E-2"/>
-                  <c:y val="-3.482575094779819E-2"/>
+                  <c:x val="-3.421432786018027E-3"/>
+                  <c:y val="-5.472363495546663E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -254,14 +262,14 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
                           <a:lumOff val="35000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
@@ -372,24 +380,14 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Pump</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Flow Rate (</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>µL/min)</a:t>
+                  <a:t>Pump Flow Rate (µL/min)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -414,7 +412,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -452,7 +450,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -499,22 +497,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Measured Flow Rate (</a:t>
+                  <a:t>Measured Flow Rate (µL/min)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>µL/min)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -538,7 +529,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -576,7 +567,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -627,7 +618,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1200,16 +1193,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>536574</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>603249</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1557,7 +1550,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>